<commit_message>
Updated RunAppReport, with new report version.
</commit_message>
<xml_diff>
--- a/examples/testproject/05 Model Files/001_Holmsdale_blkA_TM59Overheating/TM59__001_Holmsdale_blkA_TM59Overheating.xlsx
+++ b/examples/testproject/05 Model Files/001_Holmsdale_blkA_TM59Overheating/TM59__001_Holmsdale_blkA_TM59Overheating.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\engDev\git_mf\ipyrun\examples\testproject\05 Model Files\001_Holmsdale_blkA_TM59Overheating\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440DF720-B0FA-41C9-B4CD-2D08EF5F4A9F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TM59_results, air speed 0.1" sheetId="1" r:id="rId1"/>
@@ -18,12 +24,12 @@
     <sheet name="TM59_results, air speed 0.8" sheetId="9" r:id="rId9"/>
     <sheet name="TM59_results, air speed 0.2" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="43">
   <si>
     <t>Criterion A (%)</t>
   </si>
@@ -157,11 +163,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,150 +242,158 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F18" totalsRowShown="0">
-  <autoFilter ref="A1:F18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F18" totalsRowShown="0">
+  <autoFilter ref="A1:F18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Room Name"/>
-    <tableColumn id="2" name="Criterion A (%)"/>
-    <tableColumn id="3" name="Criterion A (pass/fail)"/>
-    <tableColumn id="4" name="Criterion B (%)"/>
-    <tableColumn id="5" name="Criterion B (pass/fail)"/>
-    <tableColumn id="6" name="TM59 (pass/fail)"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Room Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Criterion A (%)"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Criterion A (pass/fail)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Criterion B (%)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Criterion B (pass/fail)"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="TM59 (pass/fail)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A1:F18" totalsRowShown="0">
-  <autoFilter ref="A1:F18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table10" displayName="Table10" ref="A1:F18" totalsRowShown="0">
+  <autoFilter ref="A1:F18" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Room Name"/>
-    <tableColumn id="2" name="Criterion A (%)"/>
-    <tableColumn id="3" name="Criterion A (pass/fail)"/>
-    <tableColumn id="4" name="Criterion B (%)"/>
-    <tableColumn id="5" name="Criterion B (pass/fail)"/>
-    <tableColumn id="6" name="TM59 (pass/fail)"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Room Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Criterion A (%)"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="Criterion A (pass/fail)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="Criterion B (%)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="Criterion B (pass/fail)"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="TM59 (pass/fail)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:F18" totalsRowShown="0">
-  <autoFilter ref="A1:F18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:F18" totalsRowShown="0">
+  <autoFilter ref="A1:F18" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Room Name"/>
-    <tableColumn id="2" name="Criterion A (%)"/>
-    <tableColumn id="3" name="Criterion A (pass/fail)"/>
-    <tableColumn id="4" name="Criterion B (%)"/>
-    <tableColumn id="5" name="Criterion B (pass/fail)"/>
-    <tableColumn id="6" name="TM59 (pass/fail)"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Room Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Criterion A (%)"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Criterion A (pass/fail)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Criterion B (%)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Criterion B (pass/fail)"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="TM59 (pass/fail)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:F18" totalsRowShown="0">
-  <autoFilter ref="A1:F18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A1:F18" totalsRowShown="0">
+  <autoFilter ref="A1:F18" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Room Name"/>
-    <tableColumn id="2" name="Criterion A (%)"/>
-    <tableColumn id="3" name="Criterion A (pass/fail)"/>
-    <tableColumn id="4" name="Criterion B (%)"/>
-    <tableColumn id="5" name="Criterion B (pass/fail)"/>
-    <tableColumn id="6" name="TM59 (pass/fail)"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Room Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Criterion A (%)"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Criterion A (pass/fail)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Criterion B (%)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Criterion B (pass/fail)"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="TM59 (pass/fail)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:F18" totalsRowShown="0">
-  <autoFilter ref="A1:F18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table4" displayName="Table4" ref="A1:F18" totalsRowShown="0">
+  <autoFilter ref="A1:F18" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Room Name"/>
-    <tableColumn id="2" name="Criterion A (%)"/>
-    <tableColumn id="3" name="Criterion A (pass/fail)"/>
-    <tableColumn id="4" name="Criterion B (%)"/>
-    <tableColumn id="5" name="Criterion B (pass/fail)"/>
-    <tableColumn id="6" name="TM59 (pass/fail)"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Room Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Criterion A (%)"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Criterion A (pass/fail)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Criterion B (%)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Criterion B (pass/fail)"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="TM59 (pass/fail)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:F18" totalsRowShown="0">
-  <autoFilter ref="A1:F18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table5" displayName="Table5" ref="A1:F18" totalsRowShown="0">
+  <autoFilter ref="A1:F18" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Room Name"/>
-    <tableColumn id="2" name="Criterion A (%)"/>
-    <tableColumn id="3" name="Criterion A (pass/fail)"/>
-    <tableColumn id="4" name="Criterion B (%)"/>
-    <tableColumn id="5" name="Criterion B (pass/fail)"/>
-    <tableColumn id="6" name="TM59 (pass/fail)"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Room Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Criterion A (%)"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Criterion A (pass/fail)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Criterion B (%)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Criterion B (pass/fail)"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="TM59 (pass/fail)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:F18" totalsRowShown="0">
-  <autoFilter ref="A1:F18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table6" displayName="Table6" ref="A1:F18" totalsRowShown="0">
+  <autoFilter ref="A1:F18" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Room Name"/>
-    <tableColumn id="2" name="Criterion A (%)"/>
-    <tableColumn id="3" name="Criterion A (pass/fail)"/>
-    <tableColumn id="4" name="Criterion B (%)"/>
-    <tableColumn id="5" name="Criterion B (pass/fail)"/>
-    <tableColumn id="6" name="TM59 (pass/fail)"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Room Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Criterion A (%)"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Criterion A (pass/fail)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Criterion B (%)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Criterion B (pass/fail)"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="TM59 (pass/fail)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:F18" totalsRowShown="0">
-  <autoFilter ref="A1:F18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table7" displayName="Table7" ref="A1:F18" totalsRowShown="0">
+  <autoFilter ref="A1:F18" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Room Name"/>
-    <tableColumn id="2" name="Criterion A (%)"/>
-    <tableColumn id="3" name="Criterion A (pass/fail)"/>
-    <tableColumn id="4" name="Criterion B (%)"/>
-    <tableColumn id="5" name="Criterion B (pass/fail)"/>
-    <tableColumn id="6" name="TM59 (pass/fail)"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Room Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Criterion A (%)"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Criterion A (pass/fail)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Criterion B (%)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Criterion B (pass/fail)"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="TM59 (pass/fail)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:B9" totalsRowShown="0">
-  <autoFilter ref="A1:B9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table8" displayName="Table8" ref="A1:B9" totalsRowShown="0">
+  <autoFilter ref="A1:B9" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="index"/>
-    <tableColumn id="2" name="Column2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="index"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Column2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:F18" totalsRowShown="0">
-  <autoFilter ref="A1:F18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table9" displayName="Table9" ref="A1:F18" totalsRowShown="0">
+  <autoFilter ref="A1:F18" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Room Name"/>
-    <tableColumn id="2" name="Criterion A (%)"/>
-    <tableColumn id="3" name="Criterion A (pass/fail)"/>
-    <tableColumn id="4" name="Criterion B (%)"/>
-    <tableColumn id="5" name="Criterion B (pass/fail)"/>
-    <tableColumn id="6" name="TM59 (pass/fail)"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Room Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Criterion A (%)"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Criterion A (pass/fail)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="Criterion B (%)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="Criterion B (pass/fail)"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="TM59 (pass/fail)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -428,7 +442,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -460,9 +474,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -494,6 +526,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -669,22 +719,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="80" customHeight="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -704,12 +755,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0.804424333836098</v>
+        <v>0.80442433383609802</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
@@ -721,18 +772,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3">
-        <v>2.80501089324619</v>
+        <v>2.8050108932461901</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
       </c>
       <c r="D3">
-        <v>4.96194824961948</v>
+        <v>4.9619482496194802</v>
       </c>
       <c r="E3" t="s">
         <v>24</v>
@@ -741,12 +792,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4">
-        <v>2.77777777777778</v>
+        <v>2.7777777777777799</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
@@ -761,18 +812,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5">
-        <v>2.66884531590414</v>
+        <v>2.6688453159041399</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
       </c>
       <c r="D5">
-        <v>3.56164383561644</v>
+        <v>3.5616438356164402</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -781,12 +832,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6">
-        <v>5.48014077425842</v>
+        <v>5.4801407742584196</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
@@ -798,12 +849,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B7">
-        <v>1.45801910507793</v>
+        <v>1.4580191050779301</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
@@ -815,12 +866,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8">
-        <v>3.87129210658622</v>
+        <v>3.8712921065862198</v>
       </c>
       <c r="C8" t="s">
         <v>24</v>
@@ -832,18 +883,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B9">
-        <v>1.00762527233115</v>
+        <v>1.0076252723311501</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
       </c>
       <c r="D9">
-        <v>3.92694063926941</v>
+        <v>3.9269406392694099</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -852,7 +903,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -863,7 +914,7 @@
         <v>23</v>
       </c>
       <c r="D10">
-        <v>4.04870624048706</v>
+        <v>4.0487062404870597</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
@@ -872,7 +923,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -886,18 +937,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B12">
-        <v>6.99891067538126</v>
+        <v>6.9989106753812598</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>
       </c>
       <c r="D12">
-        <v>5.96651445966514</v>
+        <v>5.9665144596651398</v>
       </c>
       <c r="E12" t="s">
         <v>24</v>
@@ -906,18 +957,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B13">
-        <v>1.00762527233115</v>
+        <v>1.0076252723311501</v>
       </c>
       <c r="C13" t="s">
         <v>23</v>
       </c>
       <c r="D13">
-        <v>3.16590563165906</v>
+        <v>3.1659056316590601</v>
       </c>
       <c r="E13" t="s">
         <v>24</v>
@@ -926,7 +977,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -943,18 +994,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B15">
-        <v>5.85511982570806</v>
+        <v>5.8551198257080603</v>
       </c>
       <c r="C15" t="s">
         <v>24</v>
       </c>
       <c r="D15">
-        <v>6.33181126331811</v>
+        <v>6.3318112633181096</v>
       </c>
       <c r="E15" t="s">
         <v>24</v>
@@ -963,12 +1014,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B16">
-        <v>5.32931121166415</v>
+        <v>5.3293112116641499</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
@@ -980,18 +1031,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B17">
-        <v>2.64161220043573</v>
+        <v>2.6416122004357301</v>
       </c>
       <c r="C17" t="s">
         <v>23</v>
       </c>
       <c r="D17">
-        <v>4.32267884322679</v>
+        <v>4.3226788432267904</v>
       </c>
       <c r="E17" t="s">
         <v>24</v>
@@ -1000,12 +1051,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B18">
-        <v>3.97184514831574</v>
+        <v>3.9718451483157402</v>
       </c>
       <c r="C18" t="s">
         <v>24</v>
@@ -1026,7 +1077,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1036,12 +1087,12 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="80" customHeight="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1061,12 +1112,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0.0502765208647562</v>
+        <v>5.0276520864756202E-2</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
@@ -1078,18 +1129,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.217864923747277</v>
+        <v>0.21786492374727701</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
       </c>
       <c r="D3">
-        <v>4.96194824961948</v>
+        <v>4.9619482496194802</v>
       </c>
       <c r="E3" t="s">
         <v>24</v>
@@ -1098,12 +1149,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0.217864923747277</v>
+        <v>0.21786492374727701</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
@@ -1118,18 +1169,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.217864923747277</v>
+        <v>0.21786492374727701</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
       </c>
       <c r="D5">
-        <v>3.56164383561644</v>
+        <v>3.5616438356164402</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -1138,12 +1189,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6">
-        <v>1.35746606334842</v>
+        <v>1.3574660633484199</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
@@ -1155,7 +1206,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1172,12 +1223,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8">
-        <v>0.904977375565611</v>
+        <v>0.90497737556561098</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
@@ -1189,7 +1240,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1200,7 +1251,7 @@
         <v>23</v>
       </c>
       <c r="D9">
-        <v>3.92694063926941</v>
+        <v>3.9269406392694099</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -1209,18 +1260,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B10">
-        <v>0.245098039215686</v>
+        <v>0.24509803921568599</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
       </c>
       <c r="D10">
-        <v>4.07914764079148</v>
+        <v>4.0791476407914802</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
@@ -1229,7 +1280,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1243,18 +1294,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B12">
-        <v>2.61437908496732</v>
+        <v>2.6143790849673199</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
       </c>
       <c r="D12">
-        <v>5.96651445966514</v>
+        <v>5.9665144596651398</v>
       </c>
       <c r="E12" t="s">
         <v>24</v>
@@ -1263,7 +1314,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1274,7 +1325,7 @@
         <v>23</v>
       </c>
       <c r="D13">
-        <v>3.16590563165906</v>
+        <v>3.1659056316590601</v>
       </c>
       <c r="E13" t="s">
         <v>24</v>
@@ -1283,7 +1334,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1300,18 +1351,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B15">
-        <v>1.90631808278867</v>
+        <v>1.9063180827886701</v>
       </c>
       <c r="C15" t="s">
         <v>23</v>
       </c>
       <c r="D15">
-        <v>6.36225266362253</v>
+        <v>6.3622526636225301</v>
       </c>
       <c r="E15" t="s">
         <v>24</v>
@@ -1320,12 +1371,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B16">
-        <v>1.96078431372549</v>
+        <v>1.9607843137254899</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
@@ -1337,7 +1388,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1348,7 +1399,7 @@
         <v>23</v>
       </c>
       <c r="D17">
-        <v>4.32267884322679</v>
+        <v>4.3226788432267904</v>
       </c>
       <c r="E17" t="s">
         <v>24</v>
@@ -1357,12 +1408,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B18">
-        <v>0.804424333836098</v>
+        <v>0.80442433383609802</v>
       </c>
       <c r="C18" t="s">
         <v>23</v>
@@ -1383,7 +1434,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1393,12 +1444,12 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="80" customHeight="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1418,7 +1469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1435,7 +1486,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1446,7 +1497,7 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>0.852359208523592</v>
+        <v>0.85235920852359204</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
@@ -1455,7 +1506,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1466,7 +1517,7 @@
         <v>23</v>
       </c>
       <c r="D4">
-        <v>0.943683409436834</v>
+        <v>0.94368340943683404</v>
       </c>
       <c r="E4" t="s">
         <v>23</v>
@@ -1475,7 +1526,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1486,7 +1537,7 @@
         <v>23</v>
       </c>
       <c r="D5">
-        <v>0.243531202435312</v>
+        <v>0.24353120243531201</v>
       </c>
       <c r="E5" t="s">
         <v>23</v>
@@ -1495,7 +1546,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1512,7 +1563,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1529,7 +1580,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1546,7 +1597,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1557,7 +1608,7 @@
         <v>23</v>
       </c>
       <c r="D9">
-        <v>0.45662100456621</v>
+        <v>0.45662100456621002</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
@@ -1566,7 +1617,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1577,7 +1628,7 @@
         <v>23</v>
       </c>
       <c r="D10">
-        <v>0.487062404870624</v>
+        <v>0.48706240487062402</v>
       </c>
       <c r="E10" t="s">
         <v>23</v>
@@ -1586,7 +1637,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1600,7 +1651,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -1620,7 +1671,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1631,7 +1682,7 @@
         <v>23</v>
       </c>
       <c r="D13">
-        <v>0.365296803652968</v>
+        <v>0.36529680365296802</v>
       </c>
       <c r="E13" t="s">
         <v>23</v>
@@ -1640,7 +1691,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1657,7 +1708,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -1668,7 +1719,7 @@
         <v>23</v>
       </c>
       <c r="D15">
-        <v>1.15677321156773</v>
+        <v>1.1567732115677301</v>
       </c>
       <c r="E15" t="s">
         <v>24</v>
@@ -1677,7 +1728,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -1694,7 +1745,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1705,7 +1756,7 @@
         <v>23</v>
       </c>
       <c r="D17">
-        <v>0.791476407914764</v>
+        <v>0.79147640791476404</v>
       </c>
       <c r="E17" t="s">
         <v>23</v>
@@ -1714,7 +1765,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1740,7 +1791,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1750,12 +1801,12 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="80" customHeight="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1775,7 +1826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1792,7 +1843,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1812,7 +1863,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1823,7 +1874,7 @@
         <v>23</v>
       </c>
       <c r="D4">
-        <v>1.15677321156773</v>
+        <v>1.1567732115677301</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
@@ -1832,7 +1883,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1843,7 +1894,7 @@
         <v>23</v>
       </c>
       <c r="D5">
-        <v>0.547945205479452</v>
+        <v>0.54794520547945202</v>
       </c>
       <c r="E5" t="s">
         <v>23</v>
@@ -1852,7 +1903,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1869,7 +1920,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1886,7 +1937,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1903,7 +1954,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1914,7 +1965,7 @@
         <v>23</v>
       </c>
       <c r="D9">
-        <v>0.700152207001522</v>
+        <v>0.70015220700152203</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
@@ -1923,7 +1974,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1934,7 +1985,7 @@
         <v>23</v>
       </c>
       <c r="D10">
-        <v>0.76103500761035</v>
+        <v>0.76103500761035003</v>
       </c>
       <c r="E10" t="s">
         <v>23</v>
@@ -1943,7 +1994,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1957,7 +2008,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -1968,7 +2019,7 @@
         <v>23</v>
       </c>
       <c r="D12">
-        <v>1.27853881278539</v>
+        <v>1.2785388127853901</v>
       </c>
       <c r="E12" t="s">
         <v>24</v>
@@ -1977,7 +2028,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1988,7 +2039,7 @@
         <v>23</v>
       </c>
       <c r="D13">
-        <v>0.639269406392694</v>
+        <v>0.63926940639269403</v>
       </c>
       <c r="E13" t="s">
         <v>23</v>
@@ -1997,7 +2048,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -2014,7 +2065,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -2025,7 +2076,7 @@
         <v>23</v>
       </c>
       <c r="D15">
-        <v>1.46118721461187</v>
+        <v>1.4611872146118701</v>
       </c>
       <c r="E15" t="s">
         <v>24</v>
@@ -2034,7 +2085,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -2051,7 +2102,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -2062,7 +2113,7 @@
         <v>23</v>
       </c>
       <c r="D17">
-        <v>0.943683409436834</v>
+        <v>0.94368340943683404</v>
       </c>
       <c r="E17" t="s">
         <v>23</v>
@@ -2071,7 +2122,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -2097,7 +2148,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2107,12 +2158,12 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="80" customHeight="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2132,7 +2183,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2149,7 +2200,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2160,7 +2211,7 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>1.91780821917808</v>
+        <v>1.9178082191780801</v>
       </c>
       <c r="E3" t="s">
         <v>24</v>
@@ -2169,7 +2220,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2180,7 +2231,7 @@
         <v>23</v>
       </c>
       <c r="D4">
-        <v>2.07001522070015</v>
+        <v>2.0700152207001499</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
@@ -2189,7 +2240,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2200,7 +2251,7 @@
         <v>23</v>
       </c>
       <c r="D5">
-        <v>1.3089802130898</v>
+        <v>1.3089802130898001</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -2209,7 +2260,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2226,7 +2277,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -2243,7 +2294,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -2260,7 +2311,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -2271,7 +2322,7 @@
         <v>23</v>
       </c>
       <c r="D9">
-        <v>1.49162861491629</v>
+        <v>1.4916286149162901</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -2280,7 +2331,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -2291,7 +2342,7 @@
         <v>23</v>
       </c>
       <c r="D10">
-        <v>1.5220700152207</v>
+        <v>1.5220700152207001</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
@@ -2300,7 +2351,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -2314,18 +2365,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B12">
-        <v>0.0816993464052288</v>
+        <v>8.1699346405228801E-2</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
       </c>
       <c r="D12">
-        <v>2.6179604261796</v>
+        <v>2.6179604261796001</v>
       </c>
       <c r="E12" t="s">
         <v>24</v>
@@ -2334,7 +2385,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -2345,7 +2396,7 @@
         <v>23</v>
       </c>
       <c r="D13">
-        <v>1.36986301369863</v>
+        <v>1.3698630136986301</v>
       </c>
       <c r="E13" t="s">
         <v>24</v>
@@ -2354,7 +2405,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -2371,7 +2422,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -2382,7 +2433,7 @@
         <v>23</v>
       </c>
       <c r="D15">
-        <v>2.77016742770167</v>
+        <v>2.7701674277016699</v>
       </c>
       <c r="E15" t="s">
         <v>24</v>
@@ -2391,7 +2442,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -2408,7 +2459,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -2419,7 +2470,7 @@
         <v>23</v>
       </c>
       <c r="D17">
-        <v>1.67427701674277</v>
+        <v>1.6742770167427701</v>
       </c>
       <c r="E17" t="s">
         <v>24</v>
@@ -2428,7 +2479,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -2454,7 +2505,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2464,12 +2515,12 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="80" customHeight="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2489,7 +2540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2506,7 +2557,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2517,7 +2568,7 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>1.46118721461187</v>
+        <v>1.4611872146118701</v>
       </c>
       <c r="E3" t="s">
         <v>24</v>
@@ -2526,7 +2577,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2537,7 +2588,7 @@
         <v>23</v>
       </c>
       <c r="D4">
-        <v>1.55251141552511</v>
+        <v>1.5525114155251101</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
@@ -2546,7 +2597,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2557,7 +2608,7 @@
         <v>23</v>
       </c>
       <c r="D5">
-        <v>0.76103500761035</v>
+        <v>0.76103500761035003</v>
       </c>
       <c r="E5" t="s">
         <v>23</v>
@@ -2566,7 +2617,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2583,7 +2634,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -2600,7 +2651,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -2617,7 +2668,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -2628,7 +2679,7 @@
         <v>23</v>
       </c>
       <c r="D9">
-        <v>1.0958904109589</v>
+        <v>1.0958904109589001</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -2637,7 +2688,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -2657,7 +2708,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -2671,7 +2722,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -2682,7 +2733,7 @@
         <v>23</v>
       </c>
       <c r="D12">
-        <v>1.79604261796043</v>
+        <v>1.7960426179604301</v>
       </c>
       <c r="E12" t="s">
         <v>24</v>
@@ -2691,7 +2742,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -2702,7 +2753,7 @@
         <v>23</v>
       </c>
       <c r="D13">
-        <v>0.91324200913242</v>
+        <v>0.91324200913242004</v>
       </c>
       <c r="E13" t="s">
         <v>23</v>
@@ -2711,7 +2762,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -2728,7 +2779,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -2739,7 +2790,7 @@
         <v>23</v>
       </c>
       <c r="D15">
-        <v>1.88736681887367</v>
+        <v>1.8873668188736701</v>
       </c>
       <c r="E15" t="s">
         <v>24</v>
@@ -2748,7 +2799,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -2765,7 +2816,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -2776,7 +2827,7 @@
         <v>23</v>
       </c>
       <c r="D17">
-        <v>1.3089802130898</v>
+        <v>1.3089802130898001</v>
       </c>
       <c r="E17" t="s">
         <v>24</v>
@@ -2785,7 +2836,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -2811,7 +2862,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2821,12 +2872,12 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="80" customHeight="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2846,7 +2897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2863,7 +2914,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2874,7 +2925,7 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>3.01369863013699</v>
+        <v>3.0136986301369899</v>
       </c>
       <c r="E3" t="s">
         <v>24</v>
@@ -2883,7 +2934,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2894,7 +2945,7 @@
         <v>23</v>
       </c>
       <c r="D4">
-        <v>3.2572298325723</v>
+        <v>3.2572298325723001</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
@@ -2903,7 +2954,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2914,7 +2965,7 @@
         <v>23</v>
       </c>
       <c r="D5">
-        <v>2.22222222222222</v>
+        <v>2.2222222222222201</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -2923,12 +2974,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0.251382604323781</v>
+        <v>0.25138260432378101</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
@@ -2940,7 +2991,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -2957,7 +3008,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -2974,7 +3025,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -2985,7 +3036,7 @@
         <v>23</v>
       </c>
       <c r="D9">
-        <v>2.28310502283105</v>
+        <v>2.2831050228310499</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -2994,7 +3045,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -3005,7 +3056,7 @@
         <v>23</v>
       </c>
       <c r="D10">
-        <v>2.55707762557078</v>
+        <v>2.5570776255707801</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
@@ -3014,7 +3065,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -3028,18 +3079,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B12">
-        <v>0.626361655773421</v>
+        <v>0.62636165577342096</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
       </c>
       <c r="D12">
-        <v>3.95738203957382</v>
+        <v>3.9573820395738202</v>
       </c>
       <c r="E12" t="s">
         <v>24</v>
@@ -3048,7 +3099,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -3059,7 +3110,7 @@
         <v>23</v>
       </c>
       <c r="D13">
-        <v>1.91780821917808</v>
+        <v>1.9178082191780801</v>
       </c>
       <c r="E13" t="s">
         <v>24</v>
@@ -3068,7 +3119,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -3085,7 +3136,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -3105,12 +3156,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.251382604323781</v>
+        <v>0.25138260432378101</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
@@ -3122,7 +3173,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -3133,7 +3184,7 @@
         <v>23</v>
       </c>
       <c r="D17">
-        <v>2.70928462709285</v>
+        <v>2.7092846270928499</v>
       </c>
       <c r="E17" t="s">
         <v>24</v>
@@ -3142,7 +3193,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -3168,7 +3219,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3178,12 +3229,12 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="80" customHeight="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -3203,12 +3254,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0.251382604323781</v>
+        <v>0.25138260432378101</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
@@ -3220,18 +3271,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.816993464052288</v>
+        <v>0.81699346405228801</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
       </c>
       <c r="D3">
-        <v>4.96194824961948</v>
+        <v>4.9619482496194802</v>
       </c>
       <c r="E3" t="s">
         <v>24</v>
@@ -3240,18 +3291,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0.844226579520697</v>
+        <v>0.84422657952069702</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
       </c>
       <c r="D4">
-        <v>5.26636225266362</v>
+        <v>5.2663622526636198</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
@@ -3260,18 +3311,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.871459694989107</v>
+        <v>0.87145969498910703</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
       </c>
       <c r="D5">
-        <v>3.56164383561644</v>
+        <v>3.5616438356164402</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -3280,7 +3331,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -3297,7 +3348,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -3314,12 +3365,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8">
-        <v>1.96078431372549</v>
+        <v>1.9607843137254899</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
@@ -3331,18 +3382,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B9">
-        <v>0.0544662309368192</v>
+        <v>5.4466230936819203E-2</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
       </c>
       <c r="D9">
-        <v>3.92694063926941</v>
+        <v>3.9269406392694099</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -3351,18 +3402,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B10">
-        <v>0.626361655773421</v>
+        <v>0.62636165577342096</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
       </c>
       <c r="D10">
-        <v>4.07914764079148</v>
+        <v>4.0791476407914802</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
@@ -3371,7 +3422,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -3385,7 +3436,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -3396,7 +3447,7 @@
         <v>24</v>
       </c>
       <c r="D12">
-        <v>5.96651445966514</v>
+        <v>5.9665144596651398</v>
       </c>
       <c r="E12" t="s">
         <v>24</v>
@@ -3405,18 +3456,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B13">
-        <v>0.163398692810458</v>
+        <v>0.16339869281045799</v>
       </c>
       <c r="C13" t="s">
         <v>23</v>
       </c>
       <c r="D13">
-        <v>3.16590563165906</v>
+        <v>3.1659056316590601</v>
       </c>
       <c r="E13" t="s">
         <v>24</v>
@@ -3425,7 +3476,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -3442,18 +3493,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B15">
-        <v>3.48583877995643</v>
+        <v>3.4858387799564299</v>
       </c>
       <c r="C15" t="s">
         <v>24</v>
       </c>
       <c r="D15">
-        <v>6.36225266362253</v>
+        <v>6.3622526636225301</v>
       </c>
       <c r="E15" t="s">
         <v>24</v>
@@ -3462,12 +3513,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B16">
-        <v>3.11714429361488</v>
+        <v>3.1171442936148801</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
@@ -3479,18 +3530,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.925925925925926</v>
+        <v>0.92592592592592604</v>
       </c>
       <c r="C17" t="s">
         <v>23</v>
       </c>
       <c r="D17">
-        <v>4.32267884322679</v>
+        <v>4.3226788432267904</v>
       </c>
       <c r="E17" t="s">
         <v>24</v>
@@ -3499,12 +3550,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B18">
-        <v>1.96078431372549</v>
+        <v>1.9607843137254899</v>
       </c>
       <c r="C18" t="s">
         <v>23</v>
@@ -3525,7 +3576,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3535,12 +3586,12 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="80" customHeight="1">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -3548,7 +3599,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
@@ -3556,7 +3607,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
@@ -3564,7 +3615,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
@@ -3572,7 +3623,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -3580,7 +3631,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -3588,7 +3639,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
@@ -3596,7 +3647,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
@@ -3604,12 +3655,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B9" s="3">
-        <v>43999.6935693248</v>
+        <v>43999.693569324802</v>
       </c>
     </row>
   </sheetData>
@@ -3621,7 +3672,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3631,12 +3682,12 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="80" customHeight="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -3656,7 +3707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3673,7 +3724,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -3684,7 +3735,7 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>0.669710806697108</v>
+        <v>0.66971080669710803</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
@@ -3693,7 +3744,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -3704,7 +3755,7 @@
         <v>23</v>
       </c>
       <c r="D4">
-        <v>0.578386605783866</v>
+        <v>0.57838660578386603</v>
       </c>
       <c r="E4" t="s">
         <v>23</v>
@@ -3713,7 +3764,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -3724,7 +3775,7 @@
         <v>23</v>
       </c>
       <c r="D5">
-        <v>0.243531202435312</v>
+        <v>0.24353120243531201</v>
       </c>
       <c r="E5" t="s">
         <v>23</v>
@@ -3733,7 +3784,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -3750,7 +3801,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -3767,7 +3818,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -3784,7 +3835,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -3795,7 +3846,7 @@
         <v>23</v>
       </c>
       <c r="D9">
-        <v>0.273972602739726</v>
+        <v>0.27397260273972601</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
@@ -3804,7 +3855,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -3815,7 +3866,7 @@
         <v>23</v>
       </c>
       <c r="D10">
-        <v>0.30441400304414</v>
+        <v>0.30441400304414001</v>
       </c>
       <c r="E10" t="s">
         <v>23</v>
@@ -3824,7 +3875,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -3838,7 +3889,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -3849,7 +3900,7 @@
         <v>23</v>
       </c>
       <c r="D12">
-        <v>0.882800608828006</v>
+        <v>0.88280060882800604</v>
       </c>
       <c r="E12" t="s">
         <v>23</v>
@@ -3858,7 +3909,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -3869,7 +3920,7 @@
         <v>23</v>
       </c>
       <c r="D13">
-        <v>0.213089802130898</v>
+        <v>0.21308980213089801</v>
       </c>
       <c r="E13" t="s">
         <v>23</v>
@@ -3878,7 +3929,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -3895,7 +3946,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -3906,7 +3957,7 @@
         <v>23</v>
       </c>
       <c r="D15">
-        <v>0.974124809741248</v>
+        <v>0.97412480974124804</v>
       </c>
       <c r="E15" t="s">
         <v>23</v>
@@ -3915,7 +3966,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -3932,7 +3983,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -3943,7 +3994,7 @@
         <v>23</v>
       </c>
       <c r="D17">
-        <v>0.578386605783866</v>
+        <v>0.57838660578386603</v>
       </c>
       <c r="E17" t="s">
         <v>23</v>
@@ -3952,7 +4003,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>

</xml_diff>